<commit_message>
Updated the BOM kicker
</commit_message>
<xml_diff>
--- a/BOM/BOM_Kicker_Draft.xlsx
+++ b/BOM/BOM_Kicker_Draft.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\repos\SSL-Hardware-Development\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4842E0A-A01B-4621-A471-9BFF5578A6BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{991BC231-FFE9-49BB-876D-C173C91C02DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13380" xr2:uid="{F0C1FE76-4982-4239-BC71-A6B4FEE76A74}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="127">
   <si>
     <t>DA2034-ALD</t>
   </si>
@@ -405,6 +405,9 @@
   </si>
   <si>
     <t>IC FLYBACK FORW CONVERTER 10MSOP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supercapacitor </t>
   </si>
 </sst>
 </file>
@@ -584,7 +587,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -670,6 +673,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="8" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
@@ -985,10 +989,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0A1FAAE-98B2-4997-8C65-D71C62885849}">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1156,106 +1160,94 @@
       <c r="A7" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C7" s="20"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="35"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="42" t="s">
         <v>110</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C8" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D8" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="38">
+      <c r="E8" s="49">
         <v>115.46</v>
       </c>
-      <c r="F7" s="15"/>
-      <c r="G7" s="39" t="s">
+      <c r="F8" s="42"/>
+      <c r="G8" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H8" s="7">
         <v>1</v>
       </c>
-      <c r="I7" s="37" t="s">
+      <c r="I8" s="37" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="9"/>
-      <c r="B8" s="15" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="9"/>
+      <c r="B9" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C9" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="40" t="s">
+      <c r="D9" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="38">
+      <c r="E9" s="38">
         <v>19.21</v>
       </c>
-      <c r="F8" s="15"/>
-      <c r="G8" s="39" t="s">
+      <c r="F9" s="15"/>
+      <c r="G9" s="39" t="s">
         <v>118</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H9" s="7">
         <v>4</v>
       </c>
-      <c r="I8" s="36" t="s">
+      <c r="I9" s="36" t="s">
         <v>115</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="B9" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="43" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="44" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="45" t="s">
-        <v>112</v>
-      </c>
-      <c r="F9" s="42"/>
-      <c r="G9" s="46" t="s">
-        <v>117</v>
-      </c>
-      <c r="H9" s="7">
-        <v>1</v>
-      </c>
-      <c r="I9" s="21" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="22">
-        <v>7.16</v>
-      </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B10" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="F10" s="42"/>
+      <c r="G10" s="46" t="s">
         <v>117</v>
       </c>
       <c r="H10" s="7">
         <v>1</v>
       </c>
-      <c r="I10" s="7" t="s">
-        <v>114</v>
+      <c r="I10" s="21" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -1265,21 +1257,25 @@
       <c r="B11" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>24</v>
+      <c r="C11" s="21" t="s">
+        <v>21</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="47">
-        <v>10.43</v>
+        <v>23</v>
+      </c>
+      <c r="E11" s="22">
+        <v>7.16</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
+        <v>117</v>
+      </c>
+      <c r="H11" s="7">
+        <v>1</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
@@ -1288,15 +1284,19 @@
       <c r="B12" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="20" t="s">
-        <v>26</v>
+      <c r="C12" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="6"/>
+        <v>25</v>
+      </c>
+      <c r="E12" s="47">
+        <v>10.43</v>
+      </c>
       <c r="F12" s="6"/>
-      <c r="G12" s="7"/>
+      <c r="G12" s="7" t="s">
+        <v>122</v>
+      </c>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
     </row>
@@ -1307,11 +1307,11 @@
       <c r="B13" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="21" t="s">
-        <v>28</v>
+      <c r="C13" s="20" t="s">
+        <v>26</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
@@ -1324,13 +1324,13 @@
         <v>70</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>30</v>
+        <v>22</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>28</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
@@ -1342,14 +1342,14 @@
       <c r="A15" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="24" t="s">
-        <v>33</v>
+      <c r="C15" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
@@ -1358,114 +1358,108 @@
       <c r="I15" s="7"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="9"/>
+      <c r="A16" s="9" t="s">
+        <v>70</v>
+      </c>
       <c r="B16" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="C16" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="D16" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="E16" s="22">
-        <v>62.22</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" s="6"/>
       <c r="F16" s="6"/>
-      <c r="G16" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="H16" s="7">
-        <v>4</v>
-      </c>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
       <c r="I16" s="7"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="9"/>
       <c r="B17" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D17" s="26" t="s">
-        <v>95</v>
+        <v>86</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>88</v>
       </c>
       <c r="E17" s="22">
-        <v>5.29</v>
+        <v>62.22</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H17" s="7">
-        <v>2</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>94</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="I17" s="7"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="9"/>
       <c r="B18" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="C18" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="D18" s="26"/>
+      <c r="C18" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D18" s="26" t="s">
+        <v>95</v>
+      </c>
       <c r="E18" s="22">
-        <v>3.66</v>
+        <v>5.29</v>
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H18" s="7">
         <v>2</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="9"/>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="C19" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="D19" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="E19" s="29">
-        <v>216.66</v>
-      </c>
-      <c r="F19" s="7"/>
+      <c r="C19" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="D19" s="26"/>
+      <c r="E19" s="22">
+        <v>3.66</v>
+      </c>
+      <c r="F19" s="6"/>
       <c r="G19" s="7" t="s">
-        <v>17</v>
+        <v>89</v>
       </c>
       <c r="H19" s="7">
         <v>2</v>
       </c>
-      <c r="I19" s="21" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="11"/>
+      <c r="I19" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="9"/>
       <c r="B20" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="C20" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="D20" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="E20" s="31">
-        <v>9.32</v>
+        <v>72</v>
+      </c>
+      <c r="C20" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="E20" s="29">
+        <v>216.66</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="7" t="s">
@@ -1474,115 +1468,127 @@
       <c r="H20" s="7">
         <v>2</v>
       </c>
-      <c r="I20" s="7" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I20" s="21" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="11"/>
       <c r="B21" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="E21" s="31">
+        <v>9.32</v>
+      </c>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" s="7">
+        <v>2</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="11"/>
+      <c r="B22" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="C21" s="30"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-    </row>
-    <row r="22" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="11"/>
-      <c r="B22" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="C22" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="D22" s="26" t="s">
-        <v>104</v>
-      </c>
-      <c r="E22" s="33">
-        <v>8.42</v>
-      </c>
+      <c r="C22" s="30"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="31"/>
       <c r="F22" s="7"/>
-      <c r="G22" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="H22" s="7">
-        <v>4</v>
-      </c>
-      <c r="I22" s="7" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+    </row>
+    <row r="23" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="11"/>
       <c r="B23" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="C23" s="27" t="s">
-        <v>99</v>
+        <v>106</v>
+      </c>
+      <c r="C23" s="32" t="s">
+        <v>103</v>
       </c>
       <c r="D23" s="26" t="s">
-        <v>100</v>
-      </c>
-      <c r="E23" s="8">
-        <v>12.57</v>
+        <v>104</v>
+      </c>
+      <c r="E23" s="33">
+        <v>8.42</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H23" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="11"/>
-      <c r="B24" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="C24" s="30" t="s">
-        <v>84</v>
-      </c>
-      <c r="D24" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="E24" s="31">
-        <v>1.9</v>
+      <c r="B24" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="C24" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="D24" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="E24" s="8">
+        <v>12.57</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H24" s="7">
         <v>1</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A25" s="11"/>
       <c r="B25" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
+        <v>74</v>
+      </c>
+      <c r="C25" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="E25" s="31">
+        <v>1.9</v>
+      </c>
       <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
+      <c r="G25" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="H25" s="7">
+        <v>1</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="11"/>
       <c r="B26" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
@@ -1595,7 +1601,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="11"/>
       <c r="B27" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
@@ -1608,7 +1614,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="11"/>
       <c r="B28" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -1621,7 +1627,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="11"/>
       <c r="B29" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -1634,14 +1640,12 @@
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="11"/>
       <c r="B30" s="7" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
-      <c r="F30" s="7" t="s">
-        <v>81</v>
-      </c>
+      <c r="F30" s="7"/>
       <c r="G30" s="7"/>
       <c r="H30" s="7"/>
       <c r="I30" s="7"/>
@@ -1649,7 +1653,7 @@
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="11"/>
       <c r="B31" s="7" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
@@ -1663,7 +1667,9 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="11"/>
-      <c r="B32" s="7"/>
+      <c r="B32" s="7" t="s">
+        <v>80</v>
+      </c>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
@@ -1680,13 +1686,26 @@
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
+      <c r="F33" s="7" t="s">
+        <v>81</v>
+      </c>
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="7"/>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="11"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1695,22 +1714,22 @@
     <hyperlink ref="D4" r:id="rId3" display="https://www.digikey.se/en/products/detail/nextgen-components/US1M/14291100?msockid=2ae53926fc0b6a5d2b3d2c22fd5c6bda" xr:uid="{37A227CD-E31A-4F4C-A7AB-C609DEDA9238}"/>
     <hyperlink ref="D5" r:id="rId4" display="https://www.digikey.se/en/products/detail/diodes-incorporated/MURS140-13-F/814447?msockid=2ae53926fc0b6a5d2b3d2c22fd5c6bda" xr:uid="{80B17907-8465-4020-ACCA-F24F5D58E485}"/>
     <hyperlink ref="D6" r:id="rId5" xr:uid="{C7BF5BEF-988D-45F2-B8AA-2784C389B24B}"/>
-    <hyperlink ref="D7" r:id="rId6" display="https://www.mouser.se/ProductDetail/Nichicon/LGG2E182MELC45?qs=4lWw5qRttGL3gexWc5vscg%3D%3D" xr:uid="{C1BC51F4-45E1-44ED-9F12-7146C7411413}"/>
-    <hyperlink ref="D8" r:id="rId7" xr:uid="{8CAEB0A7-F876-41AD-B1DA-4608F5D01FEE}"/>
-    <hyperlink ref="D9" r:id="rId8" display="https://www.mouser.se/ProductDetail/Infineon-Technologies/IPB048N15N5LFATMA1?qs=HXFqYaX1Q2ypITzfwKA8Fg%3D%3D" xr:uid="{A0FBAA5E-CAAC-4CCE-AD06-EB5720A5C837}"/>
-    <hyperlink ref="D10" r:id="rId9" display="https://www.mouser.se/ProductDetail/Nexperia/PHT6NQ10T135?qs=LOCUfHb8d9uapm4NPa115g%3D%3D&amp;srsltid=AfmBOooTNrmQLDbKmQnQ_IS9_GgaWDTvk8lDb8iClBjMj-idlDz4wAQb&amp;_gl=1*ow4qvb*_ga*dW5kZWZpbmVk*_ga_15W4STQT4T*dW5kZWZpbmVk*_ga_1KQLCYKRX3*dW5kZWZpbmVk" xr:uid="{D8326E52-B581-4A4D-AAA4-029458EC2348}"/>
-    <hyperlink ref="D11" r:id="rId10" display="https://www.digikey.se/en/products/detail/nexperia-usa-inc/PSMN038-100YLX/4289760?msockid=2ae53926fc0b6a5d2b3d2c22fd5c6bda" xr:uid="{6F7627B7-7EAE-466F-8BDA-148F442C00AF}"/>
-    <hyperlink ref="D12" r:id="rId11" display="https://www.mouser.se/ProductDetail/Infineon-Technologies/IRF7493TRPBF?qs=9%252BKlkBgLFf1xqJe7kp9h4Q%3D%3D&amp;_gl=1*g9e4hp*_ga*MTIzMDE0NTQ5LjE3MjcyNDgxOTc.*_ga_15W4STQT4T*MTcyNzQxODUxNi4zLjAuMTcyNzQxODUxNy41OS4wLjA." xr:uid="{29665B77-6550-479F-A733-20FFA10692CE}"/>
-    <hyperlink ref="D13" r:id="rId12" display="https://www.mouser.se/ProductDetail/Infineon-Technologies/IRF6644TRPBF?qs=Z8%252BeY1k3TIJeEqdpsw%2FJmQ%3D%3D" xr:uid="{11F16CC5-7CE6-4AB8-A77F-ECB7E091AF26}"/>
-    <hyperlink ref="D14" r:id="rId13" display="https://www.elfa.se/sv/mosfet-kanal-200v-56a-to-220-infineon-irfb260npbf/p/30341315?trackQuery=MOSFET&amp;pos=5&amp;origPos=1&amp;origPageSize=50&amp;track=true&amp;filterapplied=filter_productStatus%3DAVAILABLEDELIVERY%26filter_disdrainsourcevoltagevdsnum_sv_ds%3D200&amp;sid=Ipqkdvb98c&amp;itemList=search" xr:uid="{6EA20BA0-C00C-496F-AA4D-E159ACD93EC2}"/>
-    <hyperlink ref="D15" r:id="rId14" display="https://www.elfa.se/sv/mosfet-kanal-250v-80a-to-220-ixys-ixfp80n25x3/p/30253388?trackQuery=MOSFET&amp;pos=5&amp;origPos=5&amp;origPageSize=50&amp;track=true&amp;filterapplied=filter_productStatus%3DAVAILABLEDELIVERY%26filter_disdrainsourcevoltagevdsnum_sv_ds%3D200&amp;sid=0cQN66yOSQ&amp;itemList=search" xr:uid="{3B0C98C6-CBF3-4330-9D67-79EF1981DF3B}"/>
-    <hyperlink ref="D19" r:id="rId15" xr:uid="{C97905A4-330E-BE46-B161-F43226901354}"/>
-    <hyperlink ref="D20" r:id="rId16" xr:uid="{6AC1D3F1-4921-5344-8055-C040C8F55518}"/>
-    <hyperlink ref="D24" r:id="rId17" xr:uid="{9CEFB39F-9D6A-8D44-8962-9E92291C99A6}"/>
-    <hyperlink ref="D16" r:id="rId18" display="https://www.mouser.se/ProductDetail/KEMET/CKC21C204KCGLCTU?qs=sGAEpiMZZMuMW9TJLBQkXqsU9F7klyow8n%2FTZT4NK%2FQ%3D" xr:uid="{31313F8E-E3A1-4C5A-971F-E0BAE4A2BA08}"/>
-    <hyperlink ref="D17" r:id="rId19" display="https://www.elfa.se/sv/keramisk-kondensator-10uf-25v-10-epcos-fg16x7r1e106krt06/p/30204553?pos=5&amp;origPos=1&amp;origPageSize=50&amp;track=true&amp;filterapplied=filter_discapacitancenum_sv_ds%3D0.00001&amp;sid=wzCcyDZpZg&amp;itemList=category" xr:uid="{9AFD6BDB-E80E-4388-B0FA-CE3CC10101EB}"/>
-    <hyperlink ref="D23" r:id="rId20" display="https://www.elfa.se/sv/keramisk-kondensator-47uf-25v-3216-20-epcos-c3216x5r1e476m160ac/p/30180391?pos=5&amp;origPos=15&amp;origPageSize=50&amp;track=true&amp;filterapplied=filter_productStatus%3DAVAILABLEDELIVERY%26filter_discapacitancenum_sv_ds%3D0.000047&amp;sid=zlK0Q1vsxX&amp;itemList=category" xr:uid="{9B7E4F8D-ABCC-4871-A9D6-026C6F00607F}"/>
-    <hyperlink ref="D22" r:id="rId21" display="https://www.elfa.se/sv/keramisk-kondensator-47nf-50v-10-kemet-c320c473k5r5ta7301/p/16571624?pos=5&amp;origPos=1&amp;origPageSize=50&amp;track=true&amp;filterapplied=filter_discapacitancenum_sv_ds%3D3.3e-8&amp;sid=2Pn1PYxbbl&amp;itemList=category" xr:uid="{1DC23D5B-AE9E-45E0-8E73-83E39117F711}"/>
+    <hyperlink ref="D8" r:id="rId6" display="https://www.mouser.se/ProductDetail/Nichicon/LGG2E182MELC45?qs=4lWw5qRttGL3gexWc5vscg%3D%3D" xr:uid="{C1BC51F4-45E1-44ED-9F12-7146C7411413}"/>
+    <hyperlink ref="D9" r:id="rId7" xr:uid="{8CAEB0A7-F876-41AD-B1DA-4608F5D01FEE}"/>
+    <hyperlink ref="D10" r:id="rId8" display="https://www.mouser.se/ProductDetail/Infineon-Technologies/IPB048N15N5LFATMA1?qs=HXFqYaX1Q2ypITzfwKA8Fg%3D%3D" xr:uid="{A0FBAA5E-CAAC-4CCE-AD06-EB5720A5C837}"/>
+    <hyperlink ref="D11" r:id="rId9" display="https://www.mouser.se/ProductDetail/Nexperia/PHT6NQ10T135?qs=LOCUfHb8d9uapm4NPa115g%3D%3D&amp;srsltid=AfmBOooTNrmQLDbKmQnQ_IS9_GgaWDTvk8lDb8iClBjMj-idlDz4wAQb&amp;_gl=1*ow4qvb*_ga*dW5kZWZpbmVk*_ga_15W4STQT4T*dW5kZWZpbmVk*_ga_1KQLCYKRX3*dW5kZWZpbmVk" xr:uid="{D8326E52-B581-4A4D-AAA4-029458EC2348}"/>
+    <hyperlink ref="D12" r:id="rId10" display="https://www.digikey.se/en/products/detail/nexperia-usa-inc/PSMN038-100YLX/4289760?msockid=2ae53926fc0b6a5d2b3d2c22fd5c6bda" xr:uid="{6F7627B7-7EAE-466F-8BDA-148F442C00AF}"/>
+    <hyperlink ref="D13" r:id="rId11" display="https://www.mouser.se/ProductDetail/Infineon-Technologies/IRF7493TRPBF?qs=9%252BKlkBgLFf1xqJe7kp9h4Q%3D%3D&amp;_gl=1*g9e4hp*_ga*MTIzMDE0NTQ5LjE3MjcyNDgxOTc.*_ga_15W4STQT4T*MTcyNzQxODUxNi4zLjAuMTcyNzQxODUxNy41OS4wLjA." xr:uid="{29665B77-6550-479F-A733-20FFA10692CE}"/>
+    <hyperlink ref="D14" r:id="rId12" display="https://www.mouser.se/ProductDetail/Infineon-Technologies/IRF6644TRPBF?qs=Z8%252BeY1k3TIJeEqdpsw%2FJmQ%3D%3D" xr:uid="{11F16CC5-7CE6-4AB8-A77F-ECB7E091AF26}"/>
+    <hyperlink ref="D15" r:id="rId13" display="https://www.elfa.se/sv/mosfet-kanal-200v-56a-to-220-infineon-irfb260npbf/p/30341315?trackQuery=MOSFET&amp;pos=5&amp;origPos=1&amp;origPageSize=50&amp;track=true&amp;filterapplied=filter_productStatus%3DAVAILABLEDELIVERY%26filter_disdrainsourcevoltagevdsnum_sv_ds%3D200&amp;sid=Ipqkdvb98c&amp;itemList=search" xr:uid="{6EA20BA0-C00C-496F-AA4D-E159ACD93EC2}"/>
+    <hyperlink ref="D16" r:id="rId14" display="https://www.elfa.se/sv/mosfet-kanal-250v-80a-to-220-ixys-ixfp80n25x3/p/30253388?trackQuery=MOSFET&amp;pos=5&amp;origPos=5&amp;origPageSize=50&amp;track=true&amp;filterapplied=filter_productStatus%3DAVAILABLEDELIVERY%26filter_disdrainsourcevoltagevdsnum_sv_ds%3D200&amp;sid=0cQN66yOSQ&amp;itemList=search" xr:uid="{3B0C98C6-CBF3-4330-9D67-79EF1981DF3B}"/>
+    <hyperlink ref="D20" r:id="rId15" xr:uid="{C97905A4-330E-BE46-B161-F43226901354}"/>
+    <hyperlink ref="D21" r:id="rId16" xr:uid="{6AC1D3F1-4921-5344-8055-C040C8F55518}"/>
+    <hyperlink ref="D25" r:id="rId17" xr:uid="{9CEFB39F-9D6A-8D44-8962-9E92291C99A6}"/>
+    <hyperlink ref="D17" r:id="rId18" display="https://www.mouser.se/ProductDetail/KEMET/CKC21C204KCGLCTU?qs=sGAEpiMZZMuMW9TJLBQkXqsU9F7klyow8n%2FTZT4NK%2FQ%3D" xr:uid="{31313F8E-E3A1-4C5A-971F-E0BAE4A2BA08}"/>
+    <hyperlink ref="D18" r:id="rId19" display="https://www.elfa.se/sv/keramisk-kondensator-10uf-25v-10-epcos-fg16x7r1e106krt06/p/30204553?pos=5&amp;origPos=1&amp;origPageSize=50&amp;track=true&amp;filterapplied=filter_discapacitancenum_sv_ds%3D0.00001&amp;sid=wzCcyDZpZg&amp;itemList=category" xr:uid="{9AFD6BDB-E80E-4388-B0FA-CE3CC10101EB}"/>
+    <hyperlink ref="D24" r:id="rId20" display="https://www.elfa.se/sv/keramisk-kondensator-47uf-25v-3216-20-epcos-c3216x5r1e476m160ac/p/30180391?pos=5&amp;origPos=15&amp;origPageSize=50&amp;track=true&amp;filterapplied=filter_productStatus%3DAVAILABLEDELIVERY%26filter_discapacitancenum_sv_ds%3D0.000047&amp;sid=zlK0Q1vsxX&amp;itemList=category" xr:uid="{9B7E4F8D-ABCC-4871-A9D6-026C6F00607F}"/>
+    <hyperlink ref="D23" r:id="rId21" display="https://www.elfa.se/sv/keramisk-kondensator-47nf-50v-10-kemet-c320c473k5r5ta7301/p/16571624?pos=5&amp;origPos=1&amp;origPageSize=50&amp;track=true&amp;filterapplied=filter_discapacitancenum_sv_ds%3D3.3e-8&amp;sid=2Pn1PYxbbl&amp;itemList=category" xr:uid="{1DC23D5B-AE9E-45E0-8E73-83E39117F711}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId22"/>

</xml_diff>

<commit_message>
updated the kicker bom
</commit_message>
<xml_diff>
--- a/BOM/BOM_Kicker_Draft.xlsx
+++ b/BOM/BOM_Kicker_Draft.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\repos\SSL-Hardware-Development\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5697952-BB65-4B2C-92EB-DC9BE0BBB8DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4FAB0B7-3583-47F3-84AE-8FE49340A6EF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13380" xr2:uid="{F0C1FE76-4982-4239-BC71-A6B4FEE76A74}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="138">
   <si>
     <t>DA2034-ALD</t>
   </si>
@@ -429,6 +429,18 @@
   </si>
   <si>
     <t>Capacitor 180uF</t>
+  </si>
+  <si>
+    <t>420VXG180MEFCSN25X35</t>
+  </si>
+  <si>
+    <t>Snap In</t>
+  </si>
+  <si>
+    <t>420VXG180MEFCSN25X35 Rubycon | Mouser Sverige</t>
+  </si>
+  <si>
+    <t>Capacitor 180 uF</t>
   </si>
 </sst>
 </file>
@@ -652,7 +664,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -751,13 +763,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="8" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="8" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="5" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
@@ -1073,10 +1088,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0A1FAAE-98B2-4997-8C65-D71C62885849}">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1217,20 +1232,22 @@
       <c r="A6" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="42" t="s">
-        <v>133</v>
-      </c>
-      <c r="C6" s="52" t="s">
-        <v>131</v>
-      </c>
-      <c r="D6" s="26" t="s">
-        <v>132</v>
-      </c>
-      <c r="E6" s="56">
-        <v>81.5</v>
-      </c>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
+      <c r="B6" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="C6" s="59" t="s">
+        <v>134</v>
+      </c>
+      <c r="D6" s="60" t="s">
+        <v>136</v>
+      </c>
+      <c r="E6" s="61">
+        <v>56.47</v>
+      </c>
+      <c r="F6" s="15"/>
+      <c r="G6" s="59" t="s">
+        <v>135</v>
+      </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
     </row>
@@ -1238,20 +1255,20 @@
       <c r="A7" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="51" t="s">
-        <v>129</v>
-      </c>
-      <c r="C7" s="53" t="s">
-        <v>128</v>
-      </c>
-      <c r="D7" s="59" t="s">
-        <v>130</v>
-      </c>
-      <c r="E7" s="60">
-        <v>39.25</v>
-      </c>
-      <c r="F7" s="54"/>
-      <c r="G7" s="15"/>
+      <c r="B7" s="42" t="s">
+        <v>133</v>
+      </c>
+      <c r="C7" s="52" t="s">
+        <v>131</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="E7" s="62">
+        <v>81.5</v>
+      </c>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
     </row>
@@ -1259,163 +1276,157 @@
       <c r="A8" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="57" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="58">
-        <v>155.13999999999999</v>
-      </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="H8" s="7">
-        <v>1</v>
-      </c>
-      <c r="I8" s="35" t="s">
-        <v>109</v>
-      </c>
+      <c r="B8" s="51" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" s="53" t="s">
+        <v>128</v>
+      </c>
+      <c r="D8" s="58" t="s">
+        <v>130</v>
+      </c>
+      <c r="E8" s="63">
+        <v>39.25</v>
+      </c>
+      <c r="F8" s="54"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>38</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="22"/>
+        <v>110</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="56" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="57">
+        <v>155.13999999999999</v>
+      </c>
       <c r="F9" s="6"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="35"/>
+      <c r="G9" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H9" s="7">
+        <v>1</v>
+      </c>
+      <c r="I9" s="35" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="42" t="s">
-        <v>110</v>
-      </c>
-      <c r="C10" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="49">
-        <v>115.46</v>
-      </c>
-      <c r="F10" s="42"/>
-      <c r="G10" s="46" t="s">
-        <v>118</v>
-      </c>
-      <c r="H10" s="7">
-        <v>1</v>
-      </c>
-      <c r="I10" s="37" t="s">
-        <v>109</v>
-      </c>
+      <c r="B10" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C10" s="20"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="35"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>38</v>
       </c>
       <c r="B11" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="C11" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="49">
+        <v>115.46</v>
+      </c>
+      <c r="F11" s="42"/>
+      <c r="G11" s="46" t="s">
+        <v>118</v>
+      </c>
+      <c r="H11" s="7">
+        <v>1</v>
+      </c>
+      <c r="I11" s="37" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="C11" s="43"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="50"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="9"/>
-      <c r="B12" s="15" t="s">
+      <c r="C12" s="43"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="50"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="9"/>
+      <c r="B13" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C13" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="40" t="s">
+      <c r="D13" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="38">
+      <c r="E13" s="38">
         <v>19.21</v>
       </c>
-      <c r="F12" s="15"/>
-      <c r="G12" s="39" t="s">
+      <c r="F13" s="15"/>
+      <c r="G13" s="39" t="s">
         <v>118</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H13" s="7">
         <v>4</v>
       </c>
-      <c r="I12" s="36" t="s">
+      <c r="I13" s="36" t="s">
         <v>115</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="B13" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="43" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="44" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" s="45" t="s">
-        <v>112</v>
-      </c>
-      <c r="F13" s="42"/>
-      <c r="G13" s="46" t="s">
-        <v>117</v>
-      </c>
-      <c r="H13" s="7">
-        <v>1</v>
-      </c>
-      <c r="I13" s="21" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" s="22">
-        <v>7.16</v>
-      </c>
-      <c r="F14" s="6"/>
-      <c r="G14" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B14" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="F14" s="42"/>
+      <c r="G14" s="46" t="s">
         <v>117</v>
       </c>
       <c r="H14" s="7">
         <v>1</v>
       </c>
-      <c r="I14" s="7" t="s">
-        <v>114</v>
+      <c r="I14" s="21" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -1425,21 +1436,25 @@
       <c r="B15" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>24</v>
+      <c r="C15" s="21" t="s">
+        <v>21</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" s="47">
-        <v>10.43</v>
+        <v>23</v>
+      </c>
+      <c r="E15" s="22">
+        <v>7.16</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
+        <v>117</v>
+      </c>
+      <c r="H15" s="7">
+        <v>1</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
@@ -1448,15 +1463,19 @@
       <c r="B16" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="20" t="s">
-        <v>26</v>
+      <c r="C16" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16" s="6"/>
+        <v>25</v>
+      </c>
+      <c r="E16" s="47">
+        <v>10.43</v>
+      </c>
       <c r="F16" s="6"/>
-      <c r="G16" s="7"/>
+      <c r="G16" s="7" t="s">
+        <v>122</v>
+      </c>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
     </row>
@@ -1467,11 +1486,11 @@
       <c r="B17" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="21" t="s">
-        <v>28</v>
+      <c r="C17" s="20" t="s">
+        <v>26</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
@@ -1484,13 +1503,13 @@
         <v>70</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>30</v>
+        <v>22</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>28</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
@@ -1502,14 +1521,14 @@
       <c r="A19" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="24" t="s">
-        <v>33</v>
+      <c r="C19" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
@@ -1518,114 +1537,108 @@
       <c r="I19" s="7"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="9"/>
+      <c r="A20" s="9" t="s">
+        <v>70</v>
+      </c>
       <c r="B20" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="C20" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="D20" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="E20" s="22">
-        <v>62.22</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" s="6"/>
       <c r="F20" s="6"/>
-      <c r="G20" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="H20" s="7">
-        <v>4</v>
-      </c>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
       <c r="I20" s="7"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="9"/>
       <c r="B21" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D21" s="26" t="s">
-        <v>95</v>
+        <v>86</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>88</v>
       </c>
       <c r="E21" s="22">
-        <v>5.29</v>
+        <v>62.22</v>
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H21" s="7">
-        <v>2</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>94</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="I21" s="7"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="9"/>
       <c r="B22" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="C22" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="D22" s="26"/>
+      <c r="C22" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>95</v>
+      </c>
       <c r="E22" s="22">
-        <v>3.66</v>
+        <v>5.29</v>
       </c>
       <c r="F22" s="6"/>
       <c r="G22" s="7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H22" s="7">
         <v>2</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="9"/>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="C23" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="D23" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="E23" s="29">
-        <v>216.66</v>
-      </c>
-      <c r="F23" s="7"/>
+      <c r="C23" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="D23" s="26"/>
+      <c r="E23" s="22">
+        <v>3.66</v>
+      </c>
+      <c r="F23" s="6"/>
       <c r="G23" s="7" t="s">
-        <v>17</v>
+        <v>89</v>
       </c>
       <c r="H23" s="7">
         <v>2</v>
       </c>
-      <c r="I23" s="21" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="11"/>
+      <c r="I23" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="9"/>
       <c r="B24" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="C24" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="D24" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="E24" s="31">
-        <v>9.32</v>
+        <v>72</v>
+      </c>
+      <c r="C24" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" s="29">
+        <v>216.66</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="7" t="s">
@@ -1634,115 +1647,127 @@
       <c r="H24" s="7">
         <v>2</v>
       </c>
-      <c r="I24" s="7" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I24" s="21" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A25" s="11"/>
       <c r="B25" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C25" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="E25" s="31">
+        <v>9.32</v>
+      </c>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H25" s="7">
+        <v>2</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="11"/>
+      <c r="B26" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="C25" s="30"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-    </row>
-    <row r="26" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="11"/>
-      <c r="B26" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="C26" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="D26" s="26" t="s">
-        <v>104</v>
-      </c>
-      <c r="E26" s="33">
-        <v>8.42</v>
-      </c>
+      <c r="C26" s="30"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="31"/>
       <c r="F26" s="7"/>
-      <c r="G26" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="H26" s="7">
-        <v>4</v>
-      </c>
-      <c r="I26" s="7" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+    </row>
+    <row r="27" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="11"/>
       <c r="B27" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="C27" s="27" t="s">
-        <v>99</v>
+        <v>106</v>
+      </c>
+      <c r="C27" s="32" t="s">
+        <v>103</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>100</v>
-      </c>
-      <c r="E27" s="8">
-        <v>12.57</v>
+        <v>104</v>
+      </c>
+      <c r="E27" s="33">
+        <v>8.42</v>
       </c>
       <c r="F27" s="7"/>
       <c r="G27" s="7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H27" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="11"/>
-      <c r="B28" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="C28" s="30" t="s">
-        <v>84</v>
-      </c>
-      <c r="D28" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="E28" s="31">
-        <v>1.9</v>
+      <c r="B28" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="C28" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="D28" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="E28" s="8">
+        <v>12.57</v>
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H28" s="7">
         <v>1</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A29" s="11"/>
       <c r="B29" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
+        <v>74</v>
+      </c>
+      <c r="C29" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="D29" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="E29" s="31">
+        <v>1.9</v>
+      </c>
       <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
+      <c r="G29" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="H29" s="7">
+        <v>1</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="11"/>
       <c r="B30" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
@@ -1755,7 +1780,7 @@
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="11"/>
       <c r="B31" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
@@ -1768,7 +1793,7 @@
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="11"/>
       <c r="B32" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
@@ -1781,7 +1806,7 @@
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="11"/>
       <c r="B33" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
@@ -1794,14 +1819,12 @@
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="11"/>
       <c r="B34" s="7" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
-      <c r="F34" s="7" t="s">
-        <v>81</v>
-      </c>
+      <c r="F34" s="7"/>
       <c r="G34" s="7"/>
       <c r="H34" s="7"/>
       <c r="I34" s="7"/>
@@ -1809,7 +1832,7 @@
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="11"/>
       <c r="B35" s="7" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
@@ -1823,7 +1846,9 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="11"/>
-      <c r="B36" s="7"/>
+      <c r="B36" s="7" t="s">
+        <v>80</v>
+      </c>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
@@ -1840,13 +1865,26 @@
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
+      <c r="F37" s="7" t="s">
+        <v>81</v>
+      </c>
       <c r="G37" s="7"/>
       <c r="H37" s="7"/>
       <c r="I37" s="7"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="7"/>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="11"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1854,28 +1892,29 @@
     <hyperlink ref="D2" r:id="rId2" display="https://www.digikey.se/en/products/detail/analog-devices-inc/LT3750AEMS-PBF/14683705" xr:uid="{6B11FEA2-FEE1-4B72-904F-3B1C8DE4F007}"/>
     <hyperlink ref="D4" r:id="rId3" display="https://www.digikey.se/en/products/detail/nextgen-components/US1M/14291100?msockid=2ae53926fc0b6a5d2b3d2c22fd5c6bda" xr:uid="{37A227CD-E31A-4F4C-A7AB-C609DEDA9238}"/>
     <hyperlink ref="D5" r:id="rId4" display="https://www.digikey.se/en/products/detail/diodes-incorporated/MURS140-13-F/814447?msockid=2ae53926fc0b6a5d2b3d2c22fd5c6bda" xr:uid="{80B17907-8465-4020-ACCA-F24F5D58E485}"/>
-    <hyperlink ref="D8" r:id="rId5" xr:uid="{C7BF5BEF-988D-45F2-B8AA-2784C389B24B}"/>
-    <hyperlink ref="D10" r:id="rId6" display="https://www.mouser.se/ProductDetail/Nichicon/LGG2E182MELC45?qs=4lWw5qRttGL3gexWc5vscg%3D%3D" xr:uid="{C1BC51F4-45E1-44ED-9F12-7146C7411413}"/>
-    <hyperlink ref="D12" r:id="rId7" xr:uid="{8CAEB0A7-F876-41AD-B1DA-4608F5D01FEE}"/>
-    <hyperlink ref="D13" r:id="rId8" display="https://www.mouser.se/ProductDetail/Infineon-Technologies/IPB048N15N5LFATMA1?qs=HXFqYaX1Q2ypITzfwKA8Fg%3D%3D" xr:uid="{A0FBAA5E-CAAC-4CCE-AD06-EB5720A5C837}"/>
-    <hyperlink ref="D14" r:id="rId9" display="https://www.mouser.se/ProductDetail/Nexperia/PHT6NQ10T135?qs=LOCUfHb8d9uapm4NPa115g%3D%3D&amp;srsltid=AfmBOooTNrmQLDbKmQnQ_IS9_GgaWDTvk8lDb8iClBjMj-idlDz4wAQb&amp;_gl=1*ow4qvb*_ga*dW5kZWZpbmVk*_ga_15W4STQT4T*dW5kZWZpbmVk*_ga_1KQLCYKRX3*dW5kZWZpbmVk" xr:uid="{D8326E52-B581-4A4D-AAA4-029458EC2348}"/>
-    <hyperlink ref="D15" r:id="rId10" display="https://www.digikey.se/en/products/detail/nexperia-usa-inc/PSMN038-100YLX/4289760?msockid=2ae53926fc0b6a5d2b3d2c22fd5c6bda" xr:uid="{6F7627B7-7EAE-466F-8BDA-148F442C00AF}"/>
-    <hyperlink ref="D16" r:id="rId11" display="https://www.mouser.se/ProductDetail/Infineon-Technologies/IRF7493TRPBF?qs=9%252BKlkBgLFf1xqJe7kp9h4Q%3D%3D&amp;_gl=1*g9e4hp*_ga*MTIzMDE0NTQ5LjE3MjcyNDgxOTc.*_ga_15W4STQT4T*MTcyNzQxODUxNi4zLjAuMTcyNzQxODUxNy41OS4wLjA." xr:uid="{29665B77-6550-479F-A733-20FFA10692CE}"/>
-    <hyperlink ref="D17" r:id="rId12" display="https://www.mouser.se/ProductDetail/Infineon-Technologies/IRF6644TRPBF?qs=Z8%252BeY1k3TIJeEqdpsw%2FJmQ%3D%3D" xr:uid="{11F16CC5-7CE6-4AB8-A77F-ECB7E091AF26}"/>
-    <hyperlink ref="D18" r:id="rId13" display="https://www.elfa.se/sv/mosfet-kanal-200v-56a-to-220-infineon-irfb260npbf/p/30341315?trackQuery=MOSFET&amp;pos=5&amp;origPos=1&amp;origPageSize=50&amp;track=true&amp;filterapplied=filter_productStatus%3DAVAILABLEDELIVERY%26filter_disdrainsourcevoltagevdsnum_sv_ds%3D200&amp;sid=Ipqkdvb98c&amp;itemList=search" xr:uid="{6EA20BA0-C00C-496F-AA4D-E159ACD93EC2}"/>
-    <hyperlink ref="D19" r:id="rId14" display="https://www.elfa.se/sv/mosfet-kanal-250v-80a-to-220-ixys-ixfp80n25x3/p/30253388?trackQuery=MOSFET&amp;pos=5&amp;origPos=5&amp;origPageSize=50&amp;track=true&amp;filterapplied=filter_productStatus%3DAVAILABLEDELIVERY%26filter_disdrainsourcevoltagevdsnum_sv_ds%3D200&amp;sid=0cQN66yOSQ&amp;itemList=search" xr:uid="{3B0C98C6-CBF3-4330-9D67-79EF1981DF3B}"/>
-    <hyperlink ref="D23" r:id="rId15" xr:uid="{C97905A4-330E-BE46-B161-F43226901354}"/>
-    <hyperlink ref="D24" r:id="rId16" xr:uid="{6AC1D3F1-4921-5344-8055-C040C8F55518}"/>
-    <hyperlink ref="D28" r:id="rId17" xr:uid="{9CEFB39F-9D6A-8D44-8962-9E92291C99A6}"/>
-    <hyperlink ref="D20" r:id="rId18" display="https://www.mouser.se/ProductDetail/KEMET/CKC21C204KCGLCTU?qs=sGAEpiMZZMuMW9TJLBQkXqsU9F7klyow8n%2FTZT4NK%2FQ%3D" xr:uid="{31313F8E-E3A1-4C5A-971F-E0BAE4A2BA08}"/>
-    <hyperlink ref="D21" r:id="rId19" display="https://www.elfa.se/sv/keramisk-kondensator-10uf-25v-10-epcos-fg16x7r1e106krt06/p/30204553?pos=5&amp;origPos=1&amp;origPageSize=50&amp;track=true&amp;filterapplied=filter_discapacitancenum_sv_ds%3D0.00001&amp;sid=wzCcyDZpZg&amp;itemList=category" xr:uid="{9AFD6BDB-E80E-4388-B0FA-CE3CC10101EB}"/>
-    <hyperlink ref="D27" r:id="rId20" display="https://www.elfa.se/sv/keramisk-kondensator-47uf-25v-3216-20-epcos-c3216x5r1e476m160ac/p/30180391?pos=5&amp;origPos=15&amp;origPageSize=50&amp;track=true&amp;filterapplied=filter_productStatus%3DAVAILABLEDELIVERY%26filter_discapacitancenum_sv_ds%3D0.000047&amp;sid=zlK0Q1vsxX&amp;itemList=category" xr:uid="{9B7E4F8D-ABCC-4871-A9D6-026C6F00607F}"/>
-    <hyperlink ref="D26" r:id="rId21" display="https://www.elfa.se/sv/keramisk-kondensator-47nf-50v-10-kemet-c320c473k5r5ta7301/p/16571624?pos=5&amp;origPos=1&amp;origPageSize=50&amp;track=true&amp;filterapplied=filter_discapacitancenum_sv_ds%3D3.3e-8&amp;sid=2Pn1PYxbbl&amp;itemList=category" xr:uid="{1DC23D5B-AE9E-45E0-8E73-83E39117F711}"/>
-    <hyperlink ref="D7" r:id="rId22" display="https://www.elfa.se/sv/kondensator-snap-in-220uf-20-250v-vishay-mal225753221e3/p/30179232?pos=5&amp;origPos=7&amp;origPageSize=50&amp;track=true&amp;filterapplied=filter_discapacitancenum_sv_ds%3D0.00022%26filter_disratedvoltagedcnum_sv_ds%3D250&amp;sid=iEFuCZ1HbD&amp;itemList=category" xr:uid="{9859A3AC-F96A-42AE-B28C-1C26FBF0F18C}"/>
-    <hyperlink ref="D6" r:id="rId23" display="https://www.elfa.se/sv/kondensator-snap-in-180uf-20-400v-kemet-alc80a181cb400/p/30154285?pos=5&amp;origPos=8&amp;origPageSize=50&amp;track=true&amp;filterapplied=filter_discapacitancenum_sv_ds%3D0.00018%26filter_disratedvoltagedcnum_sv_ds%3D250&amp;sid=EJ9Ia6Y9eY&amp;itemList=category" xr:uid="{2FDCF379-71FA-4044-BF37-4173185A6C6F}"/>
+    <hyperlink ref="D9" r:id="rId5" xr:uid="{C7BF5BEF-988D-45F2-B8AA-2784C389B24B}"/>
+    <hyperlink ref="D11" r:id="rId6" display="https://www.mouser.se/ProductDetail/Nichicon/LGG2E182MELC45?qs=4lWw5qRttGL3gexWc5vscg%3D%3D" xr:uid="{C1BC51F4-45E1-44ED-9F12-7146C7411413}"/>
+    <hyperlink ref="D13" r:id="rId7" xr:uid="{8CAEB0A7-F876-41AD-B1DA-4608F5D01FEE}"/>
+    <hyperlink ref="D14" r:id="rId8" display="https://www.mouser.se/ProductDetail/Infineon-Technologies/IPB048N15N5LFATMA1?qs=HXFqYaX1Q2ypITzfwKA8Fg%3D%3D" xr:uid="{A0FBAA5E-CAAC-4CCE-AD06-EB5720A5C837}"/>
+    <hyperlink ref="D15" r:id="rId9" display="https://www.mouser.se/ProductDetail/Nexperia/PHT6NQ10T135?qs=LOCUfHb8d9uapm4NPa115g%3D%3D&amp;srsltid=AfmBOooTNrmQLDbKmQnQ_IS9_GgaWDTvk8lDb8iClBjMj-idlDz4wAQb&amp;_gl=1*ow4qvb*_ga*dW5kZWZpbmVk*_ga_15W4STQT4T*dW5kZWZpbmVk*_ga_1KQLCYKRX3*dW5kZWZpbmVk" xr:uid="{D8326E52-B581-4A4D-AAA4-029458EC2348}"/>
+    <hyperlink ref="D16" r:id="rId10" display="https://www.digikey.se/en/products/detail/nexperia-usa-inc/PSMN038-100YLX/4289760?msockid=2ae53926fc0b6a5d2b3d2c22fd5c6bda" xr:uid="{6F7627B7-7EAE-466F-8BDA-148F442C00AF}"/>
+    <hyperlink ref="D17" r:id="rId11" display="https://www.mouser.se/ProductDetail/Infineon-Technologies/IRF7493TRPBF?qs=9%252BKlkBgLFf1xqJe7kp9h4Q%3D%3D&amp;_gl=1*g9e4hp*_ga*MTIzMDE0NTQ5LjE3MjcyNDgxOTc.*_ga_15W4STQT4T*MTcyNzQxODUxNi4zLjAuMTcyNzQxODUxNy41OS4wLjA." xr:uid="{29665B77-6550-479F-A733-20FFA10692CE}"/>
+    <hyperlink ref="D18" r:id="rId12" display="https://www.mouser.se/ProductDetail/Infineon-Technologies/IRF6644TRPBF?qs=Z8%252BeY1k3TIJeEqdpsw%2FJmQ%3D%3D" xr:uid="{11F16CC5-7CE6-4AB8-A77F-ECB7E091AF26}"/>
+    <hyperlink ref="D19" r:id="rId13" display="https://www.elfa.se/sv/mosfet-kanal-200v-56a-to-220-infineon-irfb260npbf/p/30341315?trackQuery=MOSFET&amp;pos=5&amp;origPos=1&amp;origPageSize=50&amp;track=true&amp;filterapplied=filter_productStatus%3DAVAILABLEDELIVERY%26filter_disdrainsourcevoltagevdsnum_sv_ds%3D200&amp;sid=Ipqkdvb98c&amp;itemList=search" xr:uid="{6EA20BA0-C00C-496F-AA4D-E159ACD93EC2}"/>
+    <hyperlink ref="D20" r:id="rId14" display="https://www.elfa.se/sv/mosfet-kanal-250v-80a-to-220-ixys-ixfp80n25x3/p/30253388?trackQuery=MOSFET&amp;pos=5&amp;origPos=5&amp;origPageSize=50&amp;track=true&amp;filterapplied=filter_productStatus%3DAVAILABLEDELIVERY%26filter_disdrainsourcevoltagevdsnum_sv_ds%3D200&amp;sid=0cQN66yOSQ&amp;itemList=search" xr:uid="{3B0C98C6-CBF3-4330-9D67-79EF1981DF3B}"/>
+    <hyperlink ref="D24" r:id="rId15" xr:uid="{C97905A4-330E-BE46-B161-F43226901354}"/>
+    <hyperlink ref="D25" r:id="rId16" xr:uid="{6AC1D3F1-4921-5344-8055-C040C8F55518}"/>
+    <hyperlink ref="D29" r:id="rId17" xr:uid="{9CEFB39F-9D6A-8D44-8962-9E92291C99A6}"/>
+    <hyperlink ref="D21" r:id="rId18" display="https://www.mouser.se/ProductDetail/KEMET/CKC21C204KCGLCTU?qs=sGAEpiMZZMuMW9TJLBQkXqsU9F7klyow8n%2FTZT4NK%2FQ%3D" xr:uid="{31313F8E-E3A1-4C5A-971F-E0BAE4A2BA08}"/>
+    <hyperlink ref="D22" r:id="rId19" display="https://www.elfa.se/sv/keramisk-kondensator-10uf-25v-10-epcos-fg16x7r1e106krt06/p/30204553?pos=5&amp;origPos=1&amp;origPageSize=50&amp;track=true&amp;filterapplied=filter_discapacitancenum_sv_ds%3D0.00001&amp;sid=wzCcyDZpZg&amp;itemList=category" xr:uid="{9AFD6BDB-E80E-4388-B0FA-CE3CC10101EB}"/>
+    <hyperlink ref="D28" r:id="rId20" display="https://www.elfa.se/sv/keramisk-kondensator-47uf-25v-3216-20-epcos-c3216x5r1e476m160ac/p/30180391?pos=5&amp;origPos=15&amp;origPageSize=50&amp;track=true&amp;filterapplied=filter_productStatus%3DAVAILABLEDELIVERY%26filter_discapacitancenum_sv_ds%3D0.000047&amp;sid=zlK0Q1vsxX&amp;itemList=category" xr:uid="{9B7E4F8D-ABCC-4871-A9D6-026C6F00607F}"/>
+    <hyperlink ref="D27" r:id="rId21" display="https://www.elfa.se/sv/keramisk-kondensator-47nf-50v-10-kemet-c320c473k5r5ta7301/p/16571624?pos=5&amp;origPos=1&amp;origPageSize=50&amp;track=true&amp;filterapplied=filter_discapacitancenum_sv_ds%3D3.3e-8&amp;sid=2Pn1PYxbbl&amp;itemList=category" xr:uid="{1DC23D5B-AE9E-45E0-8E73-83E39117F711}"/>
+    <hyperlink ref="D8" r:id="rId22" display="https://www.elfa.se/sv/kondensator-snap-in-220uf-20-250v-vishay-mal225753221e3/p/30179232?pos=5&amp;origPos=7&amp;origPageSize=50&amp;track=true&amp;filterapplied=filter_discapacitancenum_sv_ds%3D0.00022%26filter_disratedvoltagedcnum_sv_ds%3D250&amp;sid=iEFuCZ1HbD&amp;itemList=category" xr:uid="{9859A3AC-F96A-42AE-B28C-1C26FBF0F18C}"/>
+    <hyperlink ref="D7" r:id="rId23" display="https://www.elfa.se/sv/kondensator-snap-in-180uf-20-400v-kemet-alc80a181cb400/p/30154285?pos=5&amp;origPos=8&amp;origPageSize=50&amp;track=true&amp;filterapplied=filter_discapacitancenum_sv_ds%3D0.00018%26filter_disratedvoltagedcnum_sv_ds%3D250&amp;sid=EJ9Ia6Y9eY&amp;itemList=category" xr:uid="{2FDCF379-71FA-4044-BF37-4173185A6C6F}"/>
+    <hyperlink ref="D6" r:id="rId24" display="https://www.mouser.se/ProductDetail/Rubycon/420VXG180MEFCSN25X35?qs=sGAEpiMZZMvwFf0viD3Y3a3yb5D6sPUgw4mszXAf5HM5fo4Ap%2FXH5w%3D%3D" xr:uid="{8D82B597-52D6-4B32-8FF0-85551B125766}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId24"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId25"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
updated the BOM for the kicker.
</commit_message>
<xml_diff>
--- a/BOM/BOM_Kicker_Draft.xlsx
+++ b/BOM/BOM_Kicker_Draft.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\repos\SSL-Hardware-Development\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4FAB0B7-3583-47F3-84AE-8FE49340A6EF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B55778AD-E489-4462-B56F-E97CEAF1FA18}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13380" xr2:uid="{F0C1FE76-4982-4239-BC71-A6B4FEE76A74}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="139">
   <si>
     <t>DA2034-ALD</t>
   </si>
@@ -441,6 +441,9 @@
   </si>
   <si>
     <t>Capacitor 180 uF</t>
+  </si>
+  <si>
+    <t>yytrtrjtr</t>
   </si>
 </sst>
 </file>
@@ -1090,8 +1093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0A1FAAE-98B2-4997-8C65-D71C62885849}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1874,7 +1877,9 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="11"/>
-      <c r="B38" s="7"/>
+      <c r="B38" s="7" t="s">
+        <v>138</v>
+      </c>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>

</xml_diff>

<commit_message>
Added components to the BOM and updated the capacitor circuit
</commit_message>
<xml_diff>
--- a/BOM/BOM_Kicker_Draft.xlsx
+++ b/BOM/BOM_Kicker_Draft.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\repos\SSL-Hardware-Development\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB1E97F1-B156-4D57-A2C1-5A3DE1D13ABD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ADF95B3-7848-4D9D-A21F-D17C3B9E21C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13380" xr2:uid="{F0C1FE76-4982-4239-BC71-A6B4FEE76A74}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="167">
   <si>
     <t>DA2034-ALD</t>
   </si>
@@ -260,9 +260,6 @@
   </si>
   <si>
     <t>Resistor 25m</t>
-  </si>
-  <si>
-    <t>Resistor 60.4K</t>
   </si>
   <si>
     <t>Resistor 6k</t>
@@ -444,6 +441,93 @@
   </si>
   <si>
     <t xml:space="preserve">Current I </t>
+  </si>
+  <si>
+    <t>CRM2512QFX-1003ELF</t>
+  </si>
+  <si>
+    <t>CRM2512QFX-1003ELF | Bourns Motstånd, ytmontering 2W, 100kOhm, 1%, 2512 | Elfa Distrelec Sverige</t>
+  </si>
+  <si>
+    <t>Footprint</t>
+  </si>
+  <si>
+    <t>CR0603AFX-1003EAS</t>
+  </si>
+  <si>
+    <t>CR0603AFX-1003EAS | Bourns Motstånd, ytmontering 100mW, 100kOhm, 1%, 0603 | Elfa Distrelec Sverige</t>
+  </si>
+  <si>
+    <t>06 03</t>
+  </si>
+  <si>
+    <t>RC0603FR-0743RL</t>
+  </si>
+  <si>
+    <t>RC0603FR-0743RL | YAGEO Motstånd, ytmontering 100mW 43Ohm 1% 0603 | Elfa Distrelec Sverige</t>
+  </si>
+  <si>
+    <t>75V</t>
+  </si>
+  <si>
+    <t>2.0A</t>
+  </si>
+  <si>
+    <t>RMC1/16-430JTP Kamaya | Mouser Sweden</t>
+  </si>
+  <si>
+    <t>1,24 kr</t>
+  </si>
+  <si>
+    <t>RMC1/16-430JTP 5%</t>
+  </si>
+  <si>
+    <t>0.048A</t>
+  </si>
+  <si>
+    <t>ERJ-PA3J430V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resistor 43K </t>
+  </si>
+  <si>
+    <t>ERJ-PA3J430V Panasonic | Mouser Sweden</t>
+  </si>
+  <si>
+    <t>0.088A</t>
+  </si>
+  <si>
+    <t>Resistor 2.49k 1%</t>
+  </si>
+  <si>
+    <t>560112110224 | Würth Elektronik Thick Film Resistor 100mW 2.49kOhm 1% 0402 | Elfa Distrelec Sverige</t>
+  </si>
+  <si>
+    <t>04 02</t>
+  </si>
+  <si>
+    <t>50V</t>
+  </si>
+  <si>
+    <t>150V</t>
+  </si>
+  <si>
+    <t>300V</t>
+  </si>
+  <si>
+    <t>Resistor 20K</t>
+  </si>
+  <si>
+    <t>MCWR06X2491FTL</t>
+  </si>
+  <si>
+    <t>MCWR06X2491FTL - Multicomp Pro - SMD Chip Resistor, 2.49 kohm, ± 1% (farnell.com)</t>
+  </si>
+  <si>
+    <t>minimum order 10st</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;=3 </t>
   </si>
 </sst>
 </file>
@@ -453,7 +537,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;kr&quot;;[Red]\-#,##0.00\ &quot;kr&quot;"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -462,37 +546,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF333333"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF222222"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF444444"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF393E41"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -510,33 +566,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="18"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF393E41"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF393E41"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF393E41"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -544,12 +573,6 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE0E4E9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -575,8 +598,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -662,120 +691,116 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="8" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="8" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="8" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="8" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="8" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="8" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="8" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="8" fontId="5" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
@@ -1091,10 +1116,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0A1FAAE-98B2-4997-8C65-D71C62885849}">
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="C32" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1107,14 +1132,14 @@
     <col min="6" max="6" width="22.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.77734375" customWidth="1"/>
     <col min="8" max="8" width="9.77734375" customWidth="1"/>
-    <col min="9" max="9" width="15.21875" customWidth="1"/>
+    <col min="9" max="10" width="15.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C1" s="9" t="s">
@@ -1124,810 +1149,1062 @@
         <v>59</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="G1" s="48" t="s">
         <v>120</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="F1" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="I1" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="I1" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J1" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="C2" s="15" t="s">
+      <c r="B2" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="15"/>
-      <c r="F2" s="17" t="s">
+      <c r="E2" s="11"/>
+      <c r="F2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
+      <c r="G2" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="38">
+      <c r="E3" s="17">
         <v>98.56</v>
       </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F3" s="11"/>
+      <c r="G3" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="1"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E4" s="14"/>
+      <c r="F4" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="55" t="s">
+      <c r="D5" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="41">
+      <c r="E5" s="17">
         <v>4.09</v>
       </c>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F5" s="11"/>
+      <c r="G5" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="C6" s="59" t="s">
+      <c r="B6" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="E6" s="21">
+        <v>56.47</v>
+      </c>
+      <c r="F6" s="11"/>
+      <c r="G6" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="D6" s="60" t="s">
-        <v>136</v>
-      </c>
-      <c r="E6" s="61">
-        <v>56.47</v>
-      </c>
-      <c r="F6" s="15"/>
-      <c r="G6" s="59" t="s">
-        <v>135</v>
-      </c>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="42" t="s">
-        <v>133</v>
-      </c>
-      <c r="C7" s="52" t="s">
+      <c r="B7" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="D7" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="D7" s="26" t="s">
-        <v>132</v>
-      </c>
-      <c r="E7" s="62">
+      <c r="E7" s="24">
         <v>81.5</v>
       </c>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="D8" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="C8" s="53" t="s">
-        <v>128</v>
-      </c>
-      <c r="D8" s="58" t="s">
-        <v>130</v>
-      </c>
-      <c r="E8" s="63">
+      <c r="E8" s="28">
         <v>39.25</v>
       </c>
-      <c r="F8" s="54"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F8" s="29"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="C9" s="20" t="s">
+      <c r="B9" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="C9" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="56" t="s">
+      <c r="D9" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="57">
+      <c r="E9" s="32">
         <v>155.13999999999999</v>
       </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="H9" s="7">
+      <c r="F9" s="14"/>
+      <c r="G9" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="H9" s="14">
         <v>1</v>
       </c>
-      <c r="I9" s="35" t="s">
-        <v>109</v>
-      </c>
-      <c r="J9" s="7"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I9" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="35"/>
-      <c r="J10" s="7"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B10" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="C10" s="30"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="42" t="s">
-        <v>110</v>
-      </c>
-      <c r="C11" s="43" t="s">
+      <c r="B11" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="C11" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="44" t="s">
+      <c r="D11" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="49">
+      <c r="E11" s="28">
         <v>115.46</v>
       </c>
-      <c r="F11" s="42"/>
-      <c r="G11" s="46" t="s">
-        <v>118</v>
-      </c>
-      <c r="H11" s="7">
+      <c r="F11" s="22"/>
+      <c r="G11" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="H11" s="14">
         <v>1</v>
       </c>
-      <c r="I11" s="37" t="s">
-        <v>109</v>
-      </c>
-      <c r="J11" s="7"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I11" s="36" t="s">
+        <v>108</v>
+      </c>
+      <c r="J11" s="36"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="42" t="s">
-        <v>127</v>
-      </c>
-      <c r="C12" s="43"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="50"/>
-      <c r="J12" s="7"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B12" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" s="35"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="9"/>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="17">
+        <v>19.21</v>
+      </c>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="H13" s="14">
+        <v>4</v>
+      </c>
+      <c r="I13" s="39" t="s">
+        <v>114</v>
+      </c>
+      <c r="J13" s="39"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="1"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="C13" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="38">
-        <v>19.21</v>
-      </c>
-      <c r="F13" s="15"/>
-      <c r="G13" s="39" t="s">
-        <v>118</v>
-      </c>
-      <c r="H13" s="7">
-        <v>4</v>
-      </c>
-      <c r="I13" s="36" t="s">
+      <c r="F14" s="22"/>
+      <c r="G14" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="H14" s="14">
+        <v>1</v>
+      </c>
+      <c r="I14" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="J13" s="7"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="B14" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="43" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="44" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="45" t="s">
-        <v>112</v>
-      </c>
-      <c r="F14" s="42"/>
-      <c r="G14" s="46" t="s">
-        <v>117</v>
-      </c>
-      <c r="H14" s="7">
-        <v>1</v>
-      </c>
-      <c r="I14" s="21" t="s">
-        <v>116</v>
-      </c>
-      <c r="J14" s="7"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="1"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="22">
+      <c r="E15" s="34">
         <v>7.16</v>
       </c>
-      <c r="F15" s="6"/>
-      <c r="G15" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="H15" s="7">
+      <c r="F15" s="14"/>
+      <c r="G15" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="H15" s="14">
         <v>1</v>
       </c>
-      <c r="I15" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="J15" s="7"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I15" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="47">
+      <c r="E16" s="41">
         <v>10.43</v>
       </c>
-      <c r="F16" s="6"/>
-      <c r="G16" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F16" s="14"/>
+      <c r="G16" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="1"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="D17" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="1"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="21" t="s">
+      <c r="C18" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="1"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="D19" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="1"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="24" t="s">
+      <c r="C20" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="19" t="s">
+      <c r="D20" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="1"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="9"/>
-      <c r="B21" s="24" t="s">
+      <c r="B21" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="C21" s="25" t="s">
+      <c r="D21" s="44" t="s">
         <v>87</v>
       </c>
-      <c r="D21" s="23" t="s">
+      <c r="E21" s="34">
+        <v>62.22</v>
+      </c>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="E21" s="22">
-        <v>62.22</v>
-      </c>
-      <c r="F21" s="6"/>
-      <c r="G21" s="7" t="s">
+      <c r="H21" s="14">
+        <v>4</v>
+      </c>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="1"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" s="9"/>
+      <c r="B22" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="E22" s="34">
+        <v>5.29</v>
+      </c>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="H21" s="7">
+      <c r="H22" s="14">
+        <v>2</v>
+      </c>
+      <c r="I22" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="1"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" s="9"/>
+      <c r="B23" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="D23" s="18"/>
+      <c r="E23" s="34">
+        <v>3.66</v>
+      </c>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H23" s="14">
+        <v>2</v>
+      </c>
+      <c r="I23" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="J23" s="14"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="1"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" s="9"/>
+      <c r="B24" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="52" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" s="45">
+        <v>216.66</v>
+      </c>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" s="14">
+        <v>2</v>
+      </c>
+      <c r="I24" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="J24" s="14"/>
+      <c r="K24" s="14"/>
+      <c r="L24" s="1"/>
+    </row>
+    <row r="25" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="9"/>
+      <c r="B25" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C25" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="D25" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="E25" s="34">
+        <v>9.32</v>
+      </c>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H25" s="14">
+        <v>2</v>
+      </c>
+      <c r="I25" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="J25" s="14"/>
+      <c r="K25" s="14"/>
+      <c r="L25" s="1"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" s="9"/>
+      <c r="B26" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="C26" s="46"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="14"/>
+      <c r="L26" s="1"/>
+    </row>
+    <row r="27" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="9"/>
+      <c r="B27" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="C27" s="42" t="s">
+        <v>102</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="E27" s="47">
+        <v>8.42</v>
+      </c>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="H27" s="14">
         <v>4</v>
       </c>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="9"/>
-      <c r="B22" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="C22" s="6" t="s">
+      <c r="I27" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="J27" s="14"/>
+      <c r="K27" s="14"/>
+      <c r="L27" s="1"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28" s="9"/>
+      <c r="B28" s="42" t="s">
+        <v>101</v>
+      </c>
+      <c r="C28" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="E28" s="14">
+        <v>12.57</v>
+      </c>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H28" s="14">
+        <v>1</v>
+      </c>
+      <c r="I28" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="D22" s="26" t="s">
-        <v>95</v>
-      </c>
-      <c r="E22" s="22">
-        <v>5.29</v>
-      </c>
-      <c r="F22" s="6"/>
-      <c r="G22" s="7" t="s">
+      <c r="J28" s="14"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="1"/>
+    </row>
+    <row r="29" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="9"/>
+      <c r="B29" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C29" s="46" t="s">
+        <v>83</v>
+      </c>
+      <c r="D29" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="E29" s="34">
+        <v>1.9</v>
+      </c>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="H29" s="14">
+        <v>1</v>
+      </c>
+      <c r="I29" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="H22" s="7">
+      <c r="J29" s="14"/>
+      <c r="K29" s="14"/>
+      <c r="L29" s="1"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30" s="9"/>
+      <c r="B30" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E30" s="48">
+        <v>1.34</v>
+      </c>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="H30" s="14"/>
+      <c r="I30" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="J30" s="50"/>
+      <c r="K30" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="L30" s="1"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31" s="9"/>
+      <c r="B31" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E31" s="3">
+        <v>8.26</v>
+      </c>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="H31" s="14">
         <v>2</v>
       </c>
-      <c r="I22" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="J22" s="7"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="9"/>
-      <c r="B23" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="C23" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="D23" s="26"/>
-      <c r="E23" s="22">
-        <v>3.66</v>
-      </c>
-      <c r="F23" s="6"/>
-      <c r="G23" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="H23" s="7">
-        <v>2</v>
-      </c>
-      <c r="I23" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="J23" s="7"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="9"/>
-      <c r="B24" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C24" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="D24" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="E24" s="29">
-        <v>216.66</v>
-      </c>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H24" s="7">
-        <v>2</v>
-      </c>
-      <c r="I24" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="J24" s="7"/>
-    </row>
-    <row r="25" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="11"/>
-      <c r="B25" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="C25" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="D25" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="E25" s="31">
-        <v>9.32</v>
-      </c>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H25" s="7">
-        <v>2</v>
-      </c>
-      <c r="I25" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="J25" s="7"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="11"/>
-      <c r="B26" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="C26" s="30"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
-    </row>
-    <row r="27" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="11"/>
-      <c r="B27" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="C27" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="D27" s="26" t="s">
+      <c r="I31" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="J31" s="1"/>
+      <c r="K31" s="14">
+        <v>2512</v>
+      </c>
+      <c r="L31" s="1"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32" s="9"/>
+      <c r="B32" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E32" s="41">
+        <v>1.29</v>
+      </c>
+      <c r="F32" s="14"/>
+      <c r="G32" s="50"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K32" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="L32" s="1"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A33" s="9"/>
+      <c r="B33" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F33" s="14"/>
+      <c r="G33" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H33" s="14"/>
+      <c r="I33" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="E27" s="33">
-        <v>8.42</v>
-      </c>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="H27" s="7">
-        <v>4</v>
-      </c>
-      <c r="I27" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="J27" s="7"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28" s="11"/>
-      <c r="B28" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="C28" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="D28" s="26" t="s">
-        <v>100</v>
-      </c>
-      <c r="E28" s="8">
-        <v>12.57</v>
-      </c>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="H28" s="7">
+      <c r="J33" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="K33" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="L33" s="1"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A34" s="9"/>
+      <c r="B34" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E34" s="41">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="H34" s="14">
         <v>1</v>
       </c>
-      <c r="I28" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="J28" s="7"/>
-    </row>
-    <row r="29" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="11"/>
-      <c r="B29" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="C29" s="30" t="s">
-        <v>84</v>
-      </c>
-      <c r="D29" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="E29" s="31">
-        <v>1.9</v>
-      </c>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="H29" s="7">
+      <c r="I34" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="J34" s="51" t="s">
+        <v>147</v>
+      </c>
+      <c r="K34" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="L34" s="1"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A35" s="9"/>
+      <c r="B35" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="14"/>
+      <c r="J35" s="14"/>
+      <c r="K35" s="14"/>
+      <c r="L35" s="1"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A36" s="9"/>
+      <c r="B36" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="14"/>
+      <c r="J36" s="14"/>
+      <c r="K36" s="14"/>
+      <c r="L36" s="1"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A37" s="9"/>
+      <c r="B37" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="14"/>
+      <c r="J37" s="14"/>
+      <c r="K37" s="14"/>
+      <c r="L37" s="1"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A38" s="9"/>
+      <c r="B38" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="I38" s="14"/>
+      <c r="J38" s="14"/>
+      <c r="K38" s="14"/>
+      <c r="L38" s="1"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A39" s="9"/>
+      <c r="B39" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E39" s="41">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="F39" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="G39" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="H39" s="14">
+        <v>10</v>
+      </c>
+      <c r="I39" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="J39" s="14"/>
+      <c r="K39" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="L39" s="1"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A40" s="9"/>
+      <c r="B40" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="C40" s="1">
+        <v>560112110224</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E40" s="41">
+        <v>1.24</v>
+      </c>
+      <c r="F40" s="14"/>
+      <c r="G40" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H40" s="14">
         <v>1</v>
       </c>
-      <c r="I29" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="J29" s="7"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" s="11"/>
-      <c r="B30" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31" s="11"/>
-      <c r="B31" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32" s="11"/>
-      <c r="B32" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
-      <c r="J32" s="7"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A33" s="11"/>
-      <c r="B33" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="7"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A34" s="11"/>
-      <c r="B34" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
-      <c r="I34" s="7"/>
-      <c r="J34" s="7"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35" s="11"/>
-      <c r="B35" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="G35" s="7"/>
-      <c r="H35" s="7"/>
-      <c r="I35" s="7"/>
-      <c r="J35" s="7"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36" s="11"/>
-      <c r="B36" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="G36" s="7"/>
-      <c r="H36" s="7"/>
-      <c r="I36" s="7"/>
-      <c r="J36" s="7"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A37" s="11"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="G37" s="7"/>
-      <c r="H37" s="7"/>
-      <c r="I37" s="7"/>
-      <c r="J37" s="7"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A38" s="11"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
-      <c r="I38" s="7"/>
-      <c r="J38" s="7"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A41" s="7"/>
+      <c r="I40" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="J40" s="14"/>
+      <c r="K40" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="L40" s="1"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A41" s="9"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="14"/>
+      <c r="I41" s="14"/>
+      <c r="J41" s="14"/>
+      <c r="K41" s="14"/>
+      <c r="L41" s="1"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A42" s="9"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+      <c r="L42" s="1"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A43" s="9"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+      <c r="L43" s="1"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A46" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1955,9 +2232,16 @@
     <hyperlink ref="D8" r:id="rId22" display="https://www.elfa.se/sv/kondensator-snap-in-220uf-20-250v-vishay-mal225753221e3/p/30179232?pos=5&amp;origPos=7&amp;origPageSize=50&amp;track=true&amp;filterapplied=filter_discapacitancenum_sv_ds%3D0.00022%26filter_disratedvoltagedcnum_sv_ds%3D250&amp;sid=iEFuCZ1HbD&amp;itemList=category" xr:uid="{9859A3AC-F96A-42AE-B28C-1C26FBF0F18C}"/>
     <hyperlink ref="D7" r:id="rId23" display="https://www.elfa.se/sv/kondensator-snap-in-180uf-20-400v-kemet-alc80a181cb400/p/30154285?pos=5&amp;origPos=8&amp;origPageSize=50&amp;track=true&amp;filterapplied=filter_discapacitancenum_sv_ds%3D0.00018%26filter_disratedvoltagedcnum_sv_ds%3D250&amp;sid=EJ9Ia6Y9eY&amp;itemList=category" xr:uid="{2FDCF379-71FA-4044-BF37-4173185A6C6F}"/>
     <hyperlink ref="D6" r:id="rId24" display="https://www.mouser.se/ProductDetail/Rubycon/420VXG180MEFCSN25X35?qs=sGAEpiMZZMvwFf0viD3Y3a3yb5D6sPUgw4mszXAf5HM5fo4Ap%2FXH5w%3D%3D" xr:uid="{8D82B597-52D6-4B32-8FF0-85551B125766}"/>
+    <hyperlink ref="D31" r:id="rId25" display="https://www.elfa.se/sv/motstand-ytmontering-2w-100kohm-2512-bourns-crm2512qfx-1003elf/p/30388885?pos=5&amp;origPos=1&amp;origPageSize=50&amp;track=true&amp;filterapplied=filter_disvoltageratingdcnum_sv_ds%3D300%26filter_disresistancenum_sv_ds%3D100000&amp;sid=Dim1foWzXw&amp;itemList=category" xr:uid="{F39FBC53-9481-428D-B0C0-DFA0CEF8AB3F}"/>
+    <hyperlink ref="D30" r:id="rId26" display="https://www.elfa.se/sv/motstand-ytmontering-100mw-100kohm-0603-bourns-cr0603afx-1003eas/p/30388805?pos=5&amp;origPos=2&amp;origPageSize=50&amp;track=true&amp;filterapplied=filter_disvoltageratingdcnum_sv_ds%3D50%26filter_disresistancenum_sv_ds%3D100000&amp;sid=JenSR9IkBC&amp;itemList=category" xr:uid="{55777610-290F-4013-966A-CC321317F25B}"/>
+    <hyperlink ref="D34" r:id="rId27" display="https://www.elfa.se/sv/motstand-ytmontering-100mw-43ohm-0603-yageo-rc0603fr-0743rl/p/30237097?pos=5&amp;origPos=1&amp;origPageSize=50&amp;track=true&amp;filterapplied=filter_disvoltageratingdcnum_sv_ds%3D50%26filter_disresistancenum_sv_ds%3D43&amp;sid=WpROVZvcz1&amp;itemList=category" xr:uid="{4B0E4324-15AC-4750-BFE4-1CBF715B712F}"/>
+    <hyperlink ref="D33" r:id="rId28" display="https://www.mouser.se/ProductDetail/Kamaya/RMC1-16-430JTP?qs=GedFDFLaBXFDhGlKdQtZyw%3D%3D" xr:uid="{685F78AC-59FD-4235-9B5D-F7DEB1F173E9}"/>
+    <hyperlink ref="D32" r:id="rId29" display="https://www.mouser.se/ProductDetail/Panasonic/ERJ-PA3J430V?qs=BzJM0faLVqWkwxlXQtox4w%3D%3D" xr:uid="{E878A8D1-A672-460C-9ECB-1872600CB053}"/>
+    <hyperlink ref="D40" r:id="rId30" display="https://www.elfa.se/sv/thick-film-resistor-100mw-49kohm-0402-wuerth-elektronik-560112110224/p/30420414?pos=5&amp;origPos=1&amp;origPageSize=50&amp;track=true&amp;filterapplied=filter_productStatus%3DAVAILABLEDELIVERY%26filter_distoleranceplusminusnum_sv_ds%3D1%26filter_disresistancenum_sv_ds%3D2490&amp;sid=pRwzvHMjRg&amp;itemList=category" xr:uid="{DCC7C833-3231-4B9F-8DCC-4D442FBF2ED4}"/>
+    <hyperlink ref="D39" r:id="rId31" display="https://se.farnell.com/multicomp-pro/mcwr06x2491ftl/res-2k49-1-0-1w-thick-film/dp/2447323" xr:uid="{A827FD6F-D2F1-4C22-AAC5-6A73A9BCC7C3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId25"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId32"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated the BOM capacitor
</commit_message>
<xml_diff>
--- a/BOM/BOM_Kicker_Draft.xlsx
+++ b/BOM/BOM_Kicker_Draft.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\repos\SSL-Hardware-Development\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD79260-F24B-412A-83E5-0E9B089745C9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14E07E51-BF46-477F-B962-FE9C7100EEDE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13380" xr2:uid="{F0C1FE76-4982-4239-BC71-A6B4FEE76A74}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="174">
   <si>
     <t>DA2034-ALD</t>
   </si>
@@ -318,12 +318,6 @@
   </si>
   <si>
     <t>Bypass capacitor 47uF (replace the 56uF?)</t>
-  </si>
-  <si>
-    <t>C320C473K5R5TA7301</t>
-  </si>
-  <si>
-    <t>C320C473K5R5TA7301 | KEMET Keramisk kondensator, 47nF, 50V, 10% | Elfa Distrelec Sverige</t>
   </si>
   <si>
     <t xml:space="preserve">50V </t>
@@ -564,7 +558,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;kr&quot;;[Red]\-#,##0.00\ &quot;kr&quot;"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -624,6 +618,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF393E41"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF444444"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -689,7 +690,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -774,6 +775,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="8" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
@@ -1091,8 +1093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0A1FAAE-98B2-4997-8C65-D71C62885849}">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1122,25 +1124,25 @@
         <v>58</v>
       </c>
       <c r="E1" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="H1" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="F1" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>117</v>
-      </c>
       <c r="I1" s="12" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L1" s="1"/>
     </row>
@@ -1149,7 +1151,7 @@
         <v>61</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>3</v>
@@ -1162,7 +1164,7 @@
         <v>2</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H2" s="16"/>
       <c r="I2" s="16"/>
@@ -1188,7 +1190,7 @@
       </c>
       <c r="F3" s="13"/>
       <c r="G3" s="13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H3" s="16"/>
       <c r="I3" s="16"/>
@@ -1211,10 +1213,10 @@
       </c>
       <c r="E4" s="16"/>
       <c r="F4" s="16" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H4" s="16"/>
       <c r="I4" s="16"/>
@@ -1240,7 +1242,7 @@
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H5" s="16"/>
       <c r="I5" s="16"/>
@@ -1253,20 +1255,20 @@
         <v>37</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C6" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D6" s="14" t="s">
         <v>128</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>130</v>
       </c>
       <c r="E6" s="18">
         <v>56.47</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="13" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H6" s="16"/>
       <c r="I6" s="16"/>
@@ -1279,13 +1281,13 @@
         <v>37</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E7" s="37">
         <v>81.5</v>
@@ -1303,13 +1305,13 @@
         <v>37</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C8" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8" s="21" t="s">
         <v>122</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>124</v>
       </c>
       <c r="E8" s="22">
         <v>39.25</v>
@@ -1327,7 +1329,7 @@
         <v>37</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C9" s="23" t="s">
         <v>11</v>
@@ -1340,13 +1342,13 @@
       </c>
       <c r="F9" s="16"/>
       <c r="G9" s="16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H9" s="16">
         <v>1</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J9" s="16"/>
       <c r="K9" s="16"/>
@@ -1357,7 +1359,7 @@
         <v>37</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C10" s="23"/>
       <c r="D10" s="24"/>
@@ -1375,7 +1377,7 @@
         <v>37</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C11" s="26" t="s">
         <v>13</v>
@@ -1388,13 +1390,13 @@
       </c>
       <c r="F11" s="20"/>
       <c r="G11" s="20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H11" s="16">
         <v>1</v>
       </c>
       <c r="I11" s="27" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J11" s="27"/>
       <c r="K11" s="16"/>
@@ -1405,7 +1407,7 @@
         <v>37</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C12" s="26"/>
       <c r="D12" s="21"/>
@@ -1421,7 +1423,7 @@
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="12"/>
       <c r="B13" s="13" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>15</v>
@@ -1434,13 +1436,13 @@
       </c>
       <c r="F13" s="13"/>
       <c r="G13" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H13" s="16">
         <v>4</v>
       </c>
       <c r="I13" s="16" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J13" s="16"/>
       <c r="K13" s="16"/>
@@ -1448,7 +1450,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B14" s="20" t="s">
         <v>17</v>
@@ -1460,17 +1462,17 @@
         <v>19</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F14" s="20"/>
       <c r="G14" s="20" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H14" s="16">
         <v>1</v>
       </c>
       <c r="I14" s="16" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="J14" s="16"/>
       <c r="K14" s="16"/>
@@ -1494,13 +1496,13 @@
       </c>
       <c r="F15" s="16"/>
       <c r="G15" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H15" s="16">
         <v>1</v>
       </c>
       <c r="I15" s="16" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J15" s="16"/>
       <c r="K15" s="16"/>
@@ -1524,7 +1526,7 @@
       </c>
       <c r="F16" s="16"/>
       <c r="G16" s="16" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H16" s="16"/>
       <c r="I16" s="16"/>
@@ -1636,7 +1638,7 @@
       </c>
       <c r="F21" s="16"/>
       <c r="G21" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H21" s="16">
         <v>4</v>
@@ -1662,7 +1664,7 @@
       </c>
       <c r="F22" s="16"/>
       <c r="G22" s="16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H22" s="16">
         <v>2</v>
@@ -1688,7 +1690,7 @@
       </c>
       <c r="F23" s="16"/>
       <c r="G23" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H23" s="16">
         <v>2</v>
@@ -1716,7 +1718,7 @@
       </c>
       <c r="F24" s="16"/>
       <c r="G24" s="16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H24" s="16">
         <v>2</v>
@@ -1744,7 +1746,7 @@
       </c>
       <c r="F25" s="16"/>
       <c r="G25" s="16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H25" s="16">
         <v>2</v>
@@ -1775,27 +1777,15 @@
     <row r="27" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="12"/>
       <c r="B27" s="29" t="s">
-        <v>100</v>
-      </c>
-      <c r="C27" s="29" t="s">
-        <v>97</v>
-      </c>
-      <c r="D27" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="E27" s="34">
-        <v>8.42</v>
-      </c>
+      <c r="C27" s="29"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="34"/>
       <c r="F27" s="16"/>
-      <c r="G27" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="H27" s="16">
-        <v>4</v>
-      </c>
-      <c r="I27" s="16" t="s">
-        <v>99</v>
-      </c>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
       <c r="J27" s="16"/>
       <c r="K27" s="16"/>
       <c r="L27" s="1"/>
@@ -1816,7 +1806,7 @@
       </c>
       <c r="F28" s="16"/>
       <c r="G28" s="16" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H28" s="16">
         <v>1</v>
@@ -1824,7 +1814,9 @@
       <c r="I28" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="J28" s="16"/>
+      <c r="J28" s="44">
+        <v>1206</v>
+      </c>
       <c r="K28" s="16"/>
       <c r="L28" s="1"/>
     </row>
@@ -1844,7 +1836,7 @@
       </c>
       <c r="F29" s="16"/>
       <c r="G29" s="16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H29" s="16">
         <v>1</v>
@@ -1862,25 +1854,25 @@
         <v>74</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D30" s="19" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E30" s="25">
         <v>1.34</v>
       </c>
       <c r="F30" s="16"/>
       <c r="G30" s="16" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H30" s="16"/>
       <c r="I30" s="38" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J30" s="16"/>
       <c r="K30" s="16" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="L30" s="1"/>
     </row>
@@ -1890,23 +1882,23 @@
         <v>74</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D31" s="19" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E31" s="29">
         <v>8.26</v>
       </c>
       <c r="F31" s="16"/>
       <c r="G31" s="16" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H31" s="16">
         <v>2</v>
       </c>
       <c r="I31" s="16" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="J31" s="16"/>
       <c r="K31" s="16">
@@ -1917,96 +1909,96 @@
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="12"/>
       <c r="B32" s="16" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E32" s="25">
         <v>1.29</v>
       </c>
       <c r="F32" s="16"/>
       <c r="G32" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H32" s="16">
         <v>1</v>
       </c>
       <c r="I32" s="16" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="J32" s="16" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="K32" s="16" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="L32" s="1"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="12"/>
       <c r="B33" s="16" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D33" s="19" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F33" s="16"/>
       <c r="G33" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H33" s="16">
         <v>1</v>
       </c>
       <c r="I33" s="16" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J33" s="16" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="K33" s="16" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="L33" s="1"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="12"/>
       <c r="B34" s="16" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D34" s="19" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E34" s="25">
         <v>5.7000000000000002E-2</v>
       </c>
       <c r="F34" s="16"/>
       <c r="G34" s="16" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H34" s="16">
         <v>1</v>
       </c>
       <c r="I34" s="16" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="J34" s="20" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="K34" s="16" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="L34" s="1"/>
     </row>
@@ -2016,19 +2008,19 @@
         <v>75</v>
       </c>
       <c r="C35" s="40" t="s">
+        <v>167</v>
+      </c>
+      <c r="D35" s="39" t="s">
+        <v>168</v>
+      </c>
+      <c r="E35" s="41" t="s">
+        <v>166</v>
+      </c>
+      <c r="F35" s="13" t="s">
         <v>169</v>
       </c>
-      <c r="D35" s="39" t="s">
-        <v>170</v>
-      </c>
-      <c r="E35" s="41" t="s">
-        <v>168</v>
-      </c>
-      <c r="F35" s="13" t="s">
-        <v>171</v>
-      </c>
       <c r="G35" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H35" s="13">
         <v>1</v>
@@ -2044,25 +2036,25 @@
         <v>75</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E36" s="43">
         <v>5.61</v>
       </c>
       <c r="F36" s="16" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G36" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H36" s="16">
         <v>10</v>
       </c>
       <c r="I36" s="16" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="J36" s="16"/>
       <c r="K36" s="6">
@@ -2073,13 +2065,13 @@
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="12"/>
       <c r="B37" s="16" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C37" s="42" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E37" s="10">
         <v>3.64</v>
@@ -2103,7 +2095,7 @@
       </c>
       <c r="C38" s="16"/>
       <c r="D38" s="16" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E38" s="16"/>
       <c r="F38" s="16" t="s">
@@ -2111,7 +2103,7 @@
       </c>
       <c r="G38" s="16"/>
       <c r="H38" s="16" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I38" s="16"/>
       <c r="J38" s="16"/>
@@ -2121,62 +2113,62 @@
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="12"/>
       <c r="B39" s="16" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D39" s="19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E39" s="25">
         <v>0.13100000000000001</v>
       </c>
       <c r="F39" s="16" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G39" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H39" s="16">
         <v>10</v>
       </c>
       <c r="I39" s="16" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="J39" s="16"/>
       <c r="K39" s="16" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="L39" s="1"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="12"/>
       <c r="B40" s="16" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C40" s="16">
         <v>560112110224</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E40" s="25">
         <v>1.24</v>
       </c>
       <c r="F40" s="16"/>
       <c r="G40" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H40" s="16">
         <v>1</v>
       </c>
       <c r="I40" s="16" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="J40" s="16"/>
       <c r="K40" s="16" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L40" s="1"/>
     </row>
@@ -2247,23 +2239,22 @@
     <hyperlink ref="D21" r:id="rId18" display="https://www.mouser.se/ProductDetail/KEMET/CKC21C204KCGLCTU?qs=sGAEpiMZZMuMW9TJLBQkXqsU9F7klyow8n%2FTZT4NK%2FQ%3D" xr:uid="{31313F8E-E3A1-4C5A-971F-E0BAE4A2BA08}"/>
     <hyperlink ref="D22" r:id="rId19" display="https://www.elfa.se/sv/keramisk-kondensator-10uf-25v-10-epcos-fg16x7r1e106krt06/p/30204553?pos=5&amp;origPos=1&amp;origPageSize=50&amp;track=true&amp;filterapplied=filter_discapacitancenum_sv_ds%3D0.00001&amp;sid=wzCcyDZpZg&amp;itemList=category" xr:uid="{9AFD6BDB-E80E-4388-B0FA-CE3CC10101EB}"/>
     <hyperlink ref="D28" r:id="rId20" display="https://www.elfa.se/sv/keramisk-kondensator-47uf-25v-3216-20-epcos-c3216x5r1e476m160ac/p/30180391?pos=5&amp;origPos=15&amp;origPageSize=50&amp;track=true&amp;filterapplied=filter_productStatus%3DAVAILABLEDELIVERY%26filter_discapacitancenum_sv_ds%3D0.000047&amp;sid=zlK0Q1vsxX&amp;itemList=category" xr:uid="{9B7E4F8D-ABCC-4871-A9D6-026C6F00607F}"/>
-    <hyperlink ref="D27" r:id="rId21" display="https://www.elfa.se/sv/keramisk-kondensator-47nf-50v-10-kemet-c320c473k5r5ta7301/p/16571624?pos=5&amp;origPos=1&amp;origPageSize=50&amp;track=true&amp;filterapplied=filter_discapacitancenum_sv_ds%3D3.3e-8&amp;sid=2Pn1PYxbbl&amp;itemList=category" xr:uid="{1DC23D5B-AE9E-45E0-8E73-83E39117F711}"/>
-    <hyperlink ref="D8" r:id="rId22" display="https://www.elfa.se/sv/kondensator-snap-in-220uf-20-250v-vishay-mal225753221e3/p/30179232?pos=5&amp;origPos=7&amp;origPageSize=50&amp;track=true&amp;filterapplied=filter_discapacitancenum_sv_ds%3D0.00022%26filter_disratedvoltagedcnum_sv_ds%3D250&amp;sid=iEFuCZ1HbD&amp;itemList=category" xr:uid="{9859A3AC-F96A-42AE-B28C-1C26FBF0F18C}"/>
-    <hyperlink ref="D7" r:id="rId23" display="https://www.elfa.se/sv/kondensator-snap-in-180uf-20-400v-kemet-alc80a181cb400/p/30154285?pos=5&amp;origPos=8&amp;origPageSize=50&amp;track=true&amp;filterapplied=filter_discapacitancenum_sv_ds%3D0.00018%26filter_disratedvoltagedcnum_sv_ds%3D250&amp;sid=EJ9Ia6Y9eY&amp;itemList=category" xr:uid="{2FDCF379-71FA-4044-BF37-4173185A6C6F}"/>
-    <hyperlink ref="D6" r:id="rId24" display="https://www.mouser.se/ProductDetail/Rubycon/420VXG180MEFCSN25X35?qs=sGAEpiMZZMvwFf0viD3Y3a3yb5D6sPUgw4mszXAf5HM5fo4Ap%2FXH5w%3D%3D" xr:uid="{8D82B597-52D6-4B32-8FF0-85551B125766}"/>
-    <hyperlink ref="D31" r:id="rId25" display="https://www.elfa.se/sv/motstand-ytmontering-2w-100kohm-2512-bourns-crm2512qfx-1003elf/p/30388885?pos=5&amp;origPos=1&amp;origPageSize=50&amp;track=true&amp;filterapplied=filter_disvoltageratingdcnum_sv_ds%3D300%26filter_disresistancenum_sv_ds%3D100000&amp;sid=Dim1foWzXw&amp;itemList=category" xr:uid="{F39FBC53-9481-428D-B0C0-DFA0CEF8AB3F}"/>
-    <hyperlink ref="D30" r:id="rId26" display="https://www.elfa.se/sv/motstand-ytmontering-100mw-100kohm-0603-bourns-cr0603afx-1003eas/p/30388805?pos=5&amp;origPos=2&amp;origPageSize=50&amp;track=true&amp;filterapplied=filter_disvoltageratingdcnum_sv_ds%3D50%26filter_disresistancenum_sv_ds%3D100000&amp;sid=JenSR9IkBC&amp;itemList=category" xr:uid="{55777610-290F-4013-966A-CC321317F25B}"/>
-    <hyperlink ref="D34" r:id="rId27" display="https://www.elfa.se/sv/motstand-ytmontering-100mw-43ohm-0603-yageo-rc0603fr-0743rl/p/30237097?pos=5&amp;origPos=1&amp;origPageSize=50&amp;track=true&amp;filterapplied=filter_disvoltageratingdcnum_sv_ds%3D50%26filter_disresistancenum_sv_ds%3D43&amp;sid=WpROVZvcz1&amp;itemList=category" xr:uid="{4B0E4324-15AC-4750-BFE4-1CBF715B712F}"/>
-    <hyperlink ref="D33" r:id="rId28" display="https://www.mouser.se/ProductDetail/Kamaya/RMC1-16-430JTP?qs=GedFDFLaBXFDhGlKdQtZyw%3D%3D" xr:uid="{685F78AC-59FD-4235-9B5D-F7DEB1F173E9}"/>
-    <hyperlink ref="D32" r:id="rId29" display="https://www.mouser.se/ProductDetail/Panasonic/ERJ-PA3J430V?qs=BzJM0faLVqWkwxlXQtox4w%3D%3D" xr:uid="{E878A8D1-A672-460C-9ECB-1872600CB053}"/>
-    <hyperlink ref="D40" r:id="rId30" display="https://www.elfa.se/sv/thick-film-resistor-100mw-49kohm-0402-wuerth-elektronik-560112110224/p/30420414?pos=5&amp;origPos=1&amp;origPageSize=50&amp;track=true&amp;filterapplied=filter_productStatus%3DAVAILABLEDELIVERY%26filter_distoleranceplusminusnum_sv_ds%3D1%26filter_disresistancenum_sv_ds%3D2490&amp;sid=pRwzvHMjRg&amp;itemList=category" xr:uid="{DCC7C833-3231-4B9F-8DCC-4D442FBF2ED4}"/>
-    <hyperlink ref="D39" r:id="rId31" display="https://se.farnell.com/multicomp-pro/mcwr06x2491ftl/res-2k49-1-0-1w-thick-film/dp/2447323" xr:uid="{A827FD6F-D2F1-4C22-AAC5-6A73A9BCC7C3}"/>
-    <hyperlink ref="D36" r:id="rId32" display="https://se.farnell.com/multicomp-pro/mcww25wr025ftl/res-thick-film-0r025-1-2w-2512/dp/2695187" xr:uid="{F9319A3B-3EDF-42D0-847A-D4C28518C0AA}"/>
-    <hyperlink ref="D35" r:id="rId33" display="https://se.farnell.com/en-SE/ohmite/15fr025e/resistor-r025-1-5w/dp/1633926" xr:uid="{0A5644EB-4C67-4BBF-97F4-3A3D43B45830}"/>
-    <hyperlink ref="D37" r:id="rId34" display="https://www.elfa.se/sv/motstand-ytmontering-500mw-20kohm-1206-vishay-rcc120620k0fkea/p/30283294?pos=5&amp;origPos=1&amp;origPageSize=50&amp;track=true&amp;filterapplied=filter_disresistancenum_sv_ds%3D20000%26filter_dispowerratingnum_sv_ds%3D0.5&amp;sid=2u6IGmIbph&amp;itemList=category" xr:uid="{6300006B-FB8F-4EE3-88F8-29C62D75C0B4}"/>
+    <hyperlink ref="D8" r:id="rId21" display="https://www.elfa.se/sv/kondensator-snap-in-220uf-20-250v-vishay-mal225753221e3/p/30179232?pos=5&amp;origPos=7&amp;origPageSize=50&amp;track=true&amp;filterapplied=filter_discapacitancenum_sv_ds%3D0.00022%26filter_disratedvoltagedcnum_sv_ds%3D250&amp;sid=iEFuCZ1HbD&amp;itemList=category" xr:uid="{9859A3AC-F96A-42AE-B28C-1C26FBF0F18C}"/>
+    <hyperlink ref="D7" r:id="rId22" display="https://www.elfa.se/sv/kondensator-snap-in-180uf-20-400v-kemet-alc80a181cb400/p/30154285?pos=5&amp;origPos=8&amp;origPageSize=50&amp;track=true&amp;filterapplied=filter_discapacitancenum_sv_ds%3D0.00018%26filter_disratedvoltagedcnum_sv_ds%3D250&amp;sid=EJ9Ia6Y9eY&amp;itemList=category" xr:uid="{2FDCF379-71FA-4044-BF37-4173185A6C6F}"/>
+    <hyperlink ref="D6" r:id="rId23" display="https://www.mouser.se/ProductDetail/Rubycon/420VXG180MEFCSN25X35?qs=sGAEpiMZZMvwFf0viD3Y3a3yb5D6sPUgw4mszXAf5HM5fo4Ap%2FXH5w%3D%3D" xr:uid="{8D82B597-52D6-4B32-8FF0-85551B125766}"/>
+    <hyperlink ref="D31" r:id="rId24" display="https://www.elfa.se/sv/motstand-ytmontering-2w-100kohm-2512-bourns-crm2512qfx-1003elf/p/30388885?pos=5&amp;origPos=1&amp;origPageSize=50&amp;track=true&amp;filterapplied=filter_disvoltageratingdcnum_sv_ds%3D300%26filter_disresistancenum_sv_ds%3D100000&amp;sid=Dim1foWzXw&amp;itemList=category" xr:uid="{F39FBC53-9481-428D-B0C0-DFA0CEF8AB3F}"/>
+    <hyperlink ref="D30" r:id="rId25" display="https://www.elfa.se/sv/motstand-ytmontering-100mw-100kohm-0603-bourns-cr0603afx-1003eas/p/30388805?pos=5&amp;origPos=2&amp;origPageSize=50&amp;track=true&amp;filterapplied=filter_disvoltageratingdcnum_sv_ds%3D50%26filter_disresistancenum_sv_ds%3D100000&amp;sid=JenSR9IkBC&amp;itemList=category" xr:uid="{55777610-290F-4013-966A-CC321317F25B}"/>
+    <hyperlink ref="D34" r:id="rId26" display="https://www.elfa.se/sv/motstand-ytmontering-100mw-43ohm-0603-yageo-rc0603fr-0743rl/p/30237097?pos=5&amp;origPos=1&amp;origPageSize=50&amp;track=true&amp;filterapplied=filter_disvoltageratingdcnum_sv_ds%3D50%26filter_disresistancenum_sv_ds%3D43&amp;sid=WpROVZvcz1&amp;itemList=category" xr:uid="{4B0E4324-15AC-4750-BFE4-1CBF715B712F}"/>
+    <hyperlink ref="D33" r:id="rId27" display="https://www.mouser.se/ProductDetail/Kamaya/RMC1-16-430JTP?qs=GedFDFLaBXFDhGlKdQtZyw%3D%3D" xr:uid="{685F78AC-59FD-4235-9B5D-F7DEB1F173E9}"/>
+    <hyperlink ref="D32" r:id="rId28" display="https://www.mouser.se/ProductDetail/Panasonic/ERJ-PA3J430V?qs=BzJM0faLVqWkwxlXQtox4w%3D%3D" xr:uid="{E878A8D1-A672-460C-9ECB-1872600CB053}"/>
+    <hyperlink ref="D40" r:id="rId29" display="https://www.elfa.se/sv/thick-film-resistor-100mw-49kohm-0402-wuerth-elektronik-560112110224/p/30420414?pos=5&amp;origPos=1&amp;origPageSize=50&amp;track=true&amp;filterapplied=filter_productStatus%3DAVAILABLEDELIVERY%26filter_distoleranceplusminusnum_sv_ds%3D1%26filter_disresistancenum_sv_ds%3D2490&amp;sid=pRwzvHMjRg&amp;itemList=category" xr:uid="{DCC7C833-3231-4B9F-8DCC-4D442FBF2ED4}"/>
+    <hyperlink ref="D39" r:id="rId30" display="https://se.farnell.com/multicomp-pro/mcwr06x2491ftl/res-2k49-1-0-1w-thick-film/dp/2447323" xr:uid="{A827FD6F-D2F1-4C22-AAC5-6A73A9BCC7C3}"/>
+    <hyperlink ref="D36" r:id="rId31" display="https://se.farnell.com/multicomp-pro/mcww25wr025ftl/res-thick-film-0r025-1-2w-2512/dp/2695187" xr:uid="{F9319A3B-3EDF-42D0-847A-D4C28518C0AA}"/>
+    <hyperlink ref="D35" r:id="rId32" display="https://se.farnell.com/en-SE/ohmite/15fr025e/resistor-r025-1-5w/dp/1633926" xr:uid="{0A5644EB-4C67-4BBF-97F4-3A3D43B45830}"/>
+    <hyperlink ref="D37" r:id="rId33" display="https://www.elfa.se/sv/motstand-ytmontering-500mw-20kohm-1206-vishay-rcc120620k0fkea/p/30283294?pos=5&amp;origPos=1&amp;origPageSize=50&amp;track=true&amp;filterapplied=filter_disresistancenum_sv_ds%3D20000%26filter_dispowerratingnum_sv_ds%3D0.5&amp;sid=2u6IGmIbph&amp;itemList=category" xr:uid="{6300006B-FB8F-4EE3-88F8-29C62D75C0B4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId35"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId34"/>
 </worksheet>
 </file>
 

</xml_diff>